<commit_message>
updt refresh pop up
</commit_message>
<xml_diff>
--- a/output/updated_data.xlsx
+++ b/output/updated_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
   <si>
     <t>dni</t>
   </si>
@@ -58,50 +58,193 @@
     <t>institucion_3</t>
   </si>
   <si>
-    <t>07885701</t>
+    <t>46432891</t>
+  </si>
+  <si>
+    <t>70313538</t>
+  </si>
+  <si>
+    <t>71696567</t>
+  </si>
+  <si>
+    <t>72675329</t>
+  </si>
+  <si>
+    <t>32220818</t>
+  </si>
+  <si>
+    <t>32224811</t>
+  </si>
+  <si>
+    <t>75947795</t>
+  </si>
+  <si>
+    <t>72653667</t>
+  </si>
+  <si>
+    <t>70908428</t>
+  </si>
+  <si>
+    <t>70075782</t>
+  </si>
+  <si>
+    <t>70054853</t>
+  </si>
+  <si>
+    <t>77177005</t>
   </si>
   <si>
     <t>71849919</t>
   </si>
   <si>
-    <t>32220818</t>
-  </si>
-  <si>
-    <t>46432891</t>
-  </si>
-  <si>
-    <t>71696567</t>
-  </si>
-  <si>
-    <t>75947795</t>
-  </si>
-  <si>
-    <t>DARGENT BOCANEGRA, EDUARDO HERNANDO
-DNI 07885701</t>
+    <t>70326619</t>
+  </si>
+  <si>
+    <t>70219852</t>
+  </si>
+  <si>
+    <t>72674007</t>
+  </si>
+  <si>
+    <t>71474354</t>
+  </si>
+  <si>
+    <t>74832843</t>
+  </si>
+  <si>
+    <t>76910960</t>
+  </si>
+  <si>
+    <t>70793499</t>
+  </si>
+  <si>
+    <t>74396651</t>
+  </si>
+  <si>
+    <t>73505639</t>
+  </si>
+  <si>
+    <t>74237612</t>
+  </si>
+  <si>
+    <t>71269607</t>
+  </si>
+  <si>
+    <t>72765920</t>
+  </si>
+  <si>
+    <t>77225589</t>
+  </si>
+  <si>
+    <t>75904549</t>
+  </si>
+  <si>
+    <t>71594406</t>
+  </si>
+  <si>
+    <t>CALDAS VELASQUEZ, JOSUE DANIEL
+DNI 70313538</t>
+  </si>
+  <si>
+    <t>CASTILLO ESPINOZA, DARLA APRIL
+DNI 71696567</t>
+  </si>
+  <si>
+    <t>CUTIPA APAZA, ROBERTO CARLOS
+DNI 72675329</t>
+  </si>
+  <si>
+    <t>VELASQUEZ TREVEJO, SANTOS HERMELINDA
+DNI 32220818</t>
+  </si>
+  <si>
+    <t>CALDAS CAÑARI, ROMEL DAVID
+DNI 32224811</t>
+  </si>
+  <si>
+    <t>TORRES APONTE, CINDY MELISSA
+DNI 70908428</t>
+  </si>
+  <si>
+    <t>PACHAS ALMEYDA, MIGUEL ANGEL
+DNI 70075782</t>
+  </si>
+  <si>
+    <t>PEREZ PIZARRO, ORIANA LISBETH
+DNI 70054853</t>
+  </si>
+  <si>
+    <t>ARAUJO LLAMOCCA, JOAQUIN ALFONSO
+DNI 77177005</t>
   </si>
   <si>
     <t>GUZMAN UBALDO, PAMELA SOLEDAD
 DNI 71849919</t>
   </si>
   <si>
-    <t>VELASQUEZ TREVEJO, SANTOS HERMELINDA
-DNI 32220818</t>
-  </si>
-  <si>
-    <t>CASTILLO ESPINOZA, DARLA APRIL
-DNI 71696567</t>
-  </si>
-  <si>
-    <t>ABOGADO
-Fecha de diploma: 09/08/2000
-Modalidad de estudios: -</t>
-  </si>
-  <si>
-    <t>BACHILLER EN CIENCIAS CON MENCION EN INGENIERIA ECONOMICA
-Fecha de diploma: 30/11/22
-Modalidad de estudios: PRESENCIAL
-Fecha matrícula: 12/03/2015
-Fecha egreso: 19/08/2022</t>
+    <t>NAVARRO SUAREZ, ANDREA DEL CARMEN
+DNI 70326619</t>
+  </si>
+  <si>
+    <t>SAAVEDRA HIDALGO, JOSUE EDGARDO
+DNI 72674007</t>
+  </si>
+  <si>
+    <t>CHUQUITAPA HERRERA, DIEGO
+DNI 71474354</t>
+  </si>
+  <si>
+    <t>TAFUR HERNANDEZ, EMILI MARIA
+DNI 70793499</t>
+  </si>
+  <si>
+    <t>ALFERES FLORES, RUBY DARA
+DNI 74396651</t>
+  </si>
+  <si>
+    <t>CHOQUEPATA VILLANUEVA, YAMEL
+DNI 73505639</t>
+  </si>
+  <si>
+    <t>ROMERO RUEDA, DIEGO ANTONIO
+DNI 71269607</t>
+  </si>
+  <si>
+    <t>SOBRADO DE LA CRUZ, YESICA
+DNI 72765920</t>
+  </si>
+  <si>
+    <t>YAÑEZ DEL CASTILLO, MAX RICARDO
+DNI 77225589</t>
+  </si>
+  <si>
+    <t>CARBAJAL ROSAS, ALVARO JESUS
+DNI 75904549</t>
+  </si>
+  <si>
+    <t>RIVAS CERRON, CLAUDIA DANIELA
+DNI 71594406</t>
+  </si>
+  <si>
+    <t>Bachiller en Ciencias Sociales con Mención en Ciencia Política y Gobierno
+Fecha de diploma: 01/03/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 12/03/2018
+Fecha egreso: 24/01/2023</t>
+  </si>
+  <si>
+    <t>Bachiller en Ciencias Sociales con Mención en Economía
+Fecha de diploma: 01/03/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 16/03/2015
+Fecha egreso: 24/01/2023</t>
+  </si>
+  <si>
+    <t>Bachiller en Ciencias Sociales con Mención en Economía
+Fecha de diploma: 12/04/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 12/03/2018
+Fecha egreso: 24/01/2023</t>
   </si>
   <si>
     <t>LICENCIADA EN EDUCACION PRIMARIA
@@ -109,30 +252,152 @@
 Modalidad de estudios: -</t>
   </si>
   <si>
+    <t>LICENCIADO EN CIENCIAS DE LA EDUCACION
+Fecha de diploma:
+Modalidad de estudios: -</t>
+  </si>
+  <si>
+    <t>BACHILLER EN ECONOMÍA
+Fecha de diploma: 13/09/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 14/08/2017
+Fecha egreso: 03/03/2023</t>
+  </si>
+  <si>
+    <t>BACHILLER EN ECONOMIA
+Fecha de diploma: 15/03/23
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 09/03/2015
+Fecha egreso: 26/08/2022</t>
+  </si>
+  <si>
+    <t>Bachiller en Economía
+Fecha de diploma: 11/05/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 15/08/2016
+Fecha egreso: 04/08/2022</t>
+  </si>
+  <si>
+    <t>Bachiller en Ciencias Sociales con Mención en Ciencia Política y Gobierno
+Fecha de diploma: 01/03/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 13/03/2017
+Fecha egreso: 16/01/2023</t>
+  </si>
+  <si>
+    <t>BACHILLER EN CIENCIAS CON MENCION EN INGENIERIA ECONOMICA
+Fecha de diploma: 30/11/22
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 12/03/2015
+Fecha egreso: 19/08/2022</t>
+  </si>
+  <si>
+    <t>BACHILLERA EN CIENCIAS SOCIALES CON MENCIÓN EN CIENCIA POLÍTICA Y GOBIERNO
+Fecha de diploma: 04/10/23
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 12/03/2018
+Fecha egreso: 23/08/2023</t>
+  </si>
+  <si>
+    <t>BACHILLER EN ECONOMÍA
+Fecha de diploma: 30/01/23
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 17/03/2017
+Fecha egreso: 26/08/2022</t>
+  </si>
+  <si>
+    <t>TITULO PROFESIONAL DE INGENIERO DE PETROLEO Y GAS NATURAL
+Fecha de diploma: 18/08/21
+Modalidad de estudios: PRESENCIAL</t>
+  </si>
+  <si>
+    <t>BACHILLER EN CIENCIAS ECONÓMICAS
+Fecha de diploma: 20/12/22
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 06/03/2017
+Fecha egreso: 30/12/2021</t>
+  </si>
+  <si>
+    <t>Bachiller en Economía
+Fecha de diploma: 09/06/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 26/03/2018
+Fecha egreso: 30/12/2022</t>
+  </si>
+  <si>
+    <t>BACHILLER EN ECONOMÍA
+Fecha de diploma: 30/12/22
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 28/03/2017
+Fecha egreso: 30/08/2022</t>
+  </si>
+  <si>
+    <t>Bachiller en Economía y Finanzas
+Fecha de diploma: 10/05/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 19/03/2018
+Fecha egreso: 10/03/2023</t>
+  </si>
+  <si>
+    <t>Bachiller en Economía y Gestión Ambiental
+Fecha de diploma: 04/04/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 09/03/2018
+Fecha egreso: 21/12/2022</t>
+  </si>
+  <si>
+    <t>Bachiller en Ciencias Sociales con Mención en Ciencia Política y Gobierno
+Fecha de diploma: 01/03/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 12/03/2018
+Fecha egreso: 16/01/2023</t>
+  </si>
+  <si>
     <t>Bachiller en Ciencias Sociales con Mención en Economía
-Fecha de diploma: 01/03/2023
-Modalidad de estudios: PRESENCIAL
-Fecha matrícula: 16/03/2015
-Fecha egreso: 24/01/2023</t>
+Fecha de diploma: 12/04/2023
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 14/08/2017
+Fecha egreso: 16/01/2023</t>
   </si>
   <si>
     <t>PONTIFICIA UNIVERSIDAD CATÓLICA DEL PERÚ
 PERU</t>
   </si>
   <si>
+    <t>UNIVERSIDAD PRIVADA DE SAN PEDRO
+PERU</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD NACIONAL DE EDUCACIÓN ENRIQUE GUZMÁN Y VALLE
+PERU</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD NACIONAL DEL CALLAO
+PERU</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD NACIONAL MAYOR DE SAN MARCOS
+PERU</t>
+  </si>
+  <si>
     <t>UNIVERSIDAD NACIONAL DE INGENIERÍA
 PERU</t>
   </si>
   <si>
-    <t>UNIVERSIDAD PRIVADA DE SAN PEDRO
+    <t>UNIVERSIDAD NACIONAL FEDERICO VILLARREAL
 PERU</t>
   </si>
   <si>
-    <t>BACHILLER EN DERECHO
-Fecha de diploma: 02/02/2000
-Modalidad de estudios: -
-Fecha matrícula: Sin información (***)
-Fecha egreso: Sin información (***)</t>
+    <t>UNIVERSIDAD NACIONAL DE SAN AGUSTÍN DE AREQUIPA
+PERU</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD PERUANA DE CIENCIAS APLICADAS S.A.C.
+PERU</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD ANTONIO RUIZ DE MONTOYA
+PERU</t>
   </si>
   <si>
     <t>BACHILLER EN EDUCACION
@@ -142,22 +407,39 @@
 Fecha egreso: Sin información (***)</t>
   </si>
   <si>
-    <t>DOCTOR EN CIENCIA POLÍTICA Y GOBIERNO
-Fecha de diploma: 11/10/13
+    <t>LICENCIADO EN EDUCACION. ESPECIALIDAD:
+Fecha de diploma: 18/05/1998
+Modalidad de estudios: -</t>
+  </si>
+  <si>
+    <t>BACHILLER EN CIENCIAS CON MENCION EN INGENIERIA DE PETROLEO Y GAS NATURAL
+Fecha de diploma: 24/02/20
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 17/03/2014
+Fecha egreso: 09/08/2019</t>
+  </si>
+  <si>
+    <t>LICENCIADO EN CIENCIA POLÍTICA Y GOBIERNO
+Fecha de diploma: 02/08/23
+Modalidad de estudios: PRESENCIAL</t>
+  </si>
+  <si>
+    <t>BACHILLER EN CIENCIAS DE LA EDUCACION
+Fecha de diploma: 22/08/1997
 Modalidad de estudios: -
-TIPO:
-REVÁLIDA
 Fecha matrícula: Sin información (***)
 Fecha egreso: Sin información (***)</t>
   </si>
   <si>
-    <t>MASTER OF ARTS IN POLITICAL PHILOSOPHY (THE IDEA OF TOLERATION)
-Fecha de diploma:
-Modalidad de estudios: -
-TIPO:
-REVÁLIDA
-Fecha matrícula: Sin información (***)
-Fecha egreso: Sin información (***)</t>
+    <t>MAESTRO EN EDUCACION CON MENCION EN DOCENCIA UNIVERSITARIA Y GESTION EDUCATIVA
+Fecha de diploma: 12/10/17
+Modalidad de estudios: PRESENCIAL
+Fecha matrícula: 16/04/2016
+Fecha egreso: 12/11/2017</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD SAN PEDRO
+PERU</t>
   </si>
 </sst>
 </file>
@@ -515,7 +797,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -573,43 +855,7 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -623,13 +869,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -640,25 +886,16 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -669,7 +906,16 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -680,16 +926,25 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>84</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -700,7 +955,447 @@
         <v>19</v>
       </c>
       <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" t="s">
+        <v>98</v>
+      </c>
+      <c r="O7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" t="s">
+        <v>96</v>
+      </c>
+      <c r="I28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>